<commit_message>
Point and Assign Tasks
</commit_message>
<xml_diff>
--- a/Revature Room Maintenance Product Backlog.xlsx
+++ b/Revature Room Maintenance Product Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylekeck/OneDrive/Documents/project-materials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylekeck/OneDrive/Documents/iRevatureTrainingRoomMaintenanceScheduler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D25EBF-8A43-7C4F-99AD-97659C86CC42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABBEFFD-0741-2345-9D2D-838AF6FFE66E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7400" yWindow="480" windowWidth="21400" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>Totals:</t>
   </si>
@@ -174,6 +174,15 @@
   </si>
   <si>
     <t>Product Backlog -  iRevatureTrainingRoomMaintenanceScheduler</t>
+  </si>
+  <si>
+    <t>Dane</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Kyle</t>
   </si>
 </sst>
 </file>
@@ -876,7 +885,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A24" activeCellId="1" sqref="A15:A16 A24:A26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1026,9 +1037,13 @@
       <c r="C5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="16"/>
+      <c r="D5" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="E5" s="17"/>
-      <c r="F5" s="18"/>
+      <c r="F5" s="18">
+        <v>2</v>
+      </c>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
@@ -1120,9 +1135,13 @@
       <c r="C8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="16"/>
+      <c r="D8" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="E8" s="17"/>
-      <c r="F8" s="18"/>
+      <c r="F8" s="18">
+        <v>2</v>
+      </c>
       <c r="G8" s="19"/>
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
@@ -1268,9 +1287,13 @@
       <c r="C13" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="16"/>
+      <c r="D13" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="E13" s="17"/>
-      <c r="F13" s="18"/>
+      <c r="F13" s="18">
+        <v>4</v>
+      </c>
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
       <c r="I13" s="19"/>
@@ -1332,9 +1355,13 @@
       <c r="C15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="16"/>
+      <c r="D15" s="16" t="s">
+        <v>34</v>
+      </c>
       <c r="E15" s="17"/>
-      <c r="F15" s="18"/>
+      <c r="F15" s="18">
+        <v>3</v>
+      </c>
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
@@ -1396,9 +1423,13 @@
       <c r="C17" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="22"/>
+      <c r="D17" s="22" t="s">
+        <v>33</v>
+      </c>
       <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
+      <c r="F17" s="18">
+        <v>3</v>
+      </c>
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
@@ -1486,9 +1517,13 @@
       <c r="C20" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="22"/>
+      <c r="D20" s="22" t="s">
+        <v>33</v>
+      </c>
       <c r="E20" s="17"/>
-      <c r="F20" s="18"/>
+      <c r="F20" s="18">
+        <v>5</v>
+      </c>
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
       <c r="I20" s="19"/>
@@ -1606,9 +1641,13 @@
       <c r="C24" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="22"/>
+      <c r="D24" s="22" t="s">
+        <v>34</v>
+      </c>
       <c r="E24" s="17"/>
-      <c r="F24" s="18"/>
+      <c r="F24" s="18">
+        <v>4</v>
+      </c>
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
       <c r="I24" s="19"/>

</xml_diff>